<commit_message>
Added tests for verifying calculations on real map.
</commit_message>
<xml_diff>
--- a/new lat and long converter.xlsx
+++ b/new lat and long converter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e352454\dev\Projects\ads-b\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4299752-B2FF-4649-A398-0A4C3820664D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577A04B4-B8C8-4C4A-8BCF-09661757DFBE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{51E1969C-4A2B-42C5-88CD-02131A8D2726}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="32">
   <si>
     <t>Circumference of Earth (mi)</t>
   </si>
@@ -90,6 +90,42 @@
   </si>
   <si>
     <t>Miles</t>
+  </si>
+  <si>
+    <t>N7098P</t>
+  </si>
+  <si>
+    <t>(</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>)</t>
+  </si>
+  <si>
+    <t>MSQT818</t>
+  </si>
+  <si>
+    <t>N14053</t>
+  </si>
+  <si>
+    <t>MSQT955</t>
+  </si>
+  <si>
+    <t>NDU531</t>
+  </si>
+  <si>
+    <t>N94HL</t>
+  </si>
+  <si>
+    <t>*******</t>
+  </si>
+  <si>
+    <t>MSQT182</t>
+  </si>
+  <si>
+    <t>N4400Q</t>
   </si>
 </sst>
 </file>
@@ -144,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -156,6 +192,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D17263-1184-4F45-8A48-E2A233BF3566}">
-  <dimension ref="D4:U24"/>
+  <dimension ref="C4:U60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="U7" sqref="U7:U24"/>
+    <sheetView tabSelected="1" topLeftCell="B36" workbookViewId="0">
+      <selection activeCell="N60" sqref="N60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,15 +623,15 @@
         <v>-6</v>
       </c>
       <c r="S8">
-        <f t="shared" ref="S8:S24" si="0">S$6+Q8*S$4+0.01</f>
+        <f t="shared" ref="S8:S27" si="0">S$6+Q8*S$4+0.01</f>
         <v>-111.82422436405156</v>
       </c>
       <c r="T8">
-        <f t="shared" ref="T8:T24" si="1">T$6+R8*T$4+0.01</f>
+        <f t="shared" ref="T8:T27" si="1">T$6+R8*T$4+0.01</f>
         <v>33.190685495723059</v>
       </c>
       <c r="U8" t="str">
-        <f t="shared" ref="U8:U24" si="2">_xlfn.CONCAT("((",S8,",",T8,"), ""POS",P8,"""),\")</f>
+        <f t="shared" ref="U8:U27" si="2">_xlfn.CONCAT("((",S8,",",T8,"), ""POS",P8,"""),\")</f>
         <v>((-111.824224364052,33.1906854957231), "POS2"),\</v>
       </c>
     </row>
@@ -673,19 +710,19 @@
         <v>-6</v>
       </c>
       <c r="R11" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="S11" si="3">S$6+Q11*S$4+0.01</f>
         <v>-111.82422436405156</v>
       </c>
       <c r="T11">
-        <f t="shared" si="1"/>
-        <v>33.306343501425644</v>
+        <f t="shared" ref="T11" si="4">T$6+R11*T$4+0.01</f>
+        <v>33.277428999999998</v>
       </c>
       <c r="U11" t="str">
-        <f t="shared" si="2"/>
-        <v>((-111.824224364052,33.3063435014256), "POS5"),\</v>
+        <f t="shared" ref="U11" si="5">_xlfn.CONCAT("((",S11,",",T11,"), ""POS",P11,"""),\")</f>
+        <v>((-111.824224364052,33.277429), "POS5"),\</v>
       </c>
     </row>
     <row r="12" spans="4:21" x14ac:dyDescent="0.25">
@@ -696,7 +733,7 @@
         <v>-6</v>
       </c>
       <c r="R12" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S12">
         <f t="shared" si="0"/>
@@ -704,11 +741,11 @@
       </c>
       <c r="T12">
         <f t="shared" si="1"/>
-        <v>33.33525800285129</v>
+        <v>33.306343501425644</v>
       </c>
       <c r="U12" t="str">
         <f t="shared" si="2"/>
-        <v>((-111.824224364052,33.3352580028513), "POS6"),\</v>
+        <v>((-111.824224364052,33.3063435014256), "POS6"),\</v>
       </c>
     </row>
     <row r="13" spans="4:21" x14ac:dyDescent="0.25">
@@ -733,14 +770,14 @@
         <v>7</v>
       </c>
       <c r="Q13" s="3">
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="R13" s="3">
         <v>4</v>
       </c>
       <c r="S13">
         <f t="shared" si="0"/>
-        <v>-111.78964257603437</v>
+        <v>-111.82422436405156</v>
       </c>
       <c r="T13">
         <f t="shared" si="1"/>
@@ -748,7 +785,7 @@
       </c>
       <c r="U13" t="str">
         <f t="shared" si="2"/>
-        <v>((-111.789642576034,33.3352580028513), "POS7"),\</v>
+        <v>((-111.824224364052,33.3352580028513), "POS7"),\</v>
       </c>
     </row>
     <row r="14" spans="4:21" x14ac:dyDescent="0.25">
@@ -773,14 +810,14 @@
         <v>8</v>
       </c>
       <c r="Q14" s="3">
-        <v>-2</v>
+        <v>-4</v>
       </c>
       <c r="R14" s="3">
         <v>4</v>
       </c>
       <c r="S14">
         <f t="shared" si="0"/>
-        <v>-111.75506078801719</v>
+        <v>-111.78964257603437</v>
       </c>
       <c r="T14">
         <f t="shared" si="1"/>
@@ -788,7 +825,7 @@
       </c>
       <c r="U14" t="str">
         <f t="shared" si="2"/>
-        <v>((-111.755060788017,33.3352580028513), "POS8"),\</v>
+        <v>((-111.789642576034,33.3352580028513), "POS8"),\</v>
       </c>
     </row>
     <row r="15" spans="4:21" x14ac:dyDescent="0.25">
@@ -813,14 +850,14 @@
         <v>9</v>
       </c>
       <c r="Q15" s="3">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="R15" s="3">
         <v>4</v>
       </c>
       <c r="S15">
         <f t="shared" si="0"/>
-        <v>-111.68589721198281</v>
+        <v>-111.75506078801719</v>
       </c>
       <c r="T15">
         <f t="shared" si="1"/>
@@ -828,7 +865,7 @@
       </c>
       <c r="U15" t="str">
         <f t="shared" si="2"/>
-        <v>((-111.685897211983,33.3352580028513), "POS9"),\</v>
+        <v>((-111.755060788017,33.3352580028513), "POS9"),\</v>
       </c>
     </row>
     <row r="16" spans="4:21" x14ac:dyDescent="0.25">
@@ -856,22 +893,22 @@
         <v>10</v>
       </c>
       <c r="Q16" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="R16" s="3">
         <v>4</v>
       </c>
       <c r="S16">
-        <f t="shared" si="0"/>
-        <v>-111.65131542396563</v>
+        <f t="shared" ref="S16" si="6">S$6+Q16*S$4+0.01</f>
+        <v>-111.720479</v>
       </c>
       <c r="T16">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="T16" si="7">T$6+R16*T$4+0.01</f>
         <v>33.33525800285129</v>
       </c>
       <c r="U16" t="str">
-        <f t="shared" si="2"/>
-        <v>((-111.651315423966,33.3352580028513), "POS10"),\</v>
+        <f t="shared" ref="U16" si="8">_xlfn.CONCAT("((",S16,",",T16,"), ""POS",P16,"""),\")</f>
+        <v>((-111.720479,33.3352580028513), "POS10"),\</v>
       </c>
     </row>
     <row r="17" spans="4:21" x14ac:dyDescent="0.25">
@@ -900,14 +937,14 @@
         <v>11</v>
       </c>
       <c r="Q17" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="R17" s="3">
         <v>4</v>
       </c>
       <c r="S17">
         <f t="shared" si="0"/>
-        <v>-111.61673363594844</v>
+        <v>-111.68589721198281</v>
       </c>
       <c r="T17">
         <f t="shared" si="1"/>
@@ -915,7 +952,7 @@
       </c>
       <c r="U17" t="str">
         <f t="shared" si="2"/>
-        <v>((-111.616733635948,33.3352580028513), "POS11"),\</v>
+        <v>((-111.685897211983,33.3352580028513), "POS11"),\</v>
       </c>
     </row>
     <row r="18" spans="4:21" x14ac:dyDescent="0.25">
@@ -927,22 +964,22 @@
         <v>12</v>
       </c>
       <c r="Q18" s="3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="R18" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S18">
         <f t="shared" si="0"/>
-        <v>-111.61673363594844</v>
+        <v>-111.65131542396563</v>
       </c>
       <c r="T18">
         <f t="shared" si="1"/>
-        <v>33.306343501425644</v>
+        <v>33.33525800285129</v>
       </c>
       <c r="U18" t="str">
         <f t="shared" si="2"/>
-        <v>((-111.616733635948,33.3063435014256), "POS12"),\</v>
+        <v>((-111.651315423966,33.3352580028513), "POS12"),\</v>
       </c>
     </row>
     <row r="19" spans="4:21" x14ac:dyDescent="0.25">
@@ -957,7 +994,7 @@
         <v>6</v>
       </c>
       <c r="R19" s="3">
-        <v>-2</v>
+        <v>4</v>
       </c>
       <c r="S19">
         <f t="shared" si="0"/>
@@ -965,11 +1002,11 @@
       </c>
       <c r="T19">
         <f t="shared" si="1"/>
-        <v>33.248514498574352</v>
+        <v>33.33525800285129</v>
       </c>
       <c r="U19" t="str">
         <f t="shared" si="2"/>
-        <v>((-111.616733635948,33.2485144985744), "POS13"),\</v>
+        <v>((-111.616733635948,33.3352580028513), "POS13"),\</v>
       </c>
     </row>
     <row r="20" spans="4:21" x14ac:dyDescent="0.25">
@@ -984,7 +1021,7 @@
         <v>6</v>
       </c>
       <c r="R20" s="3">
-        <v>-4</v>
+        <v>2</v>
       </c>
       <c r="S20">
         <f t="shared" si="0"/>
@@ -992,11 +1029,11 @@
       </c>
       <c r="T20">
         <f t="shared" si="1"/>
-        <v>33.219599997148705</v>
+        <v>33.306343501425644</v>
       </c>
       <c r="U20" t="str">
         <f t="shared" si="2"/>
-        <v>((-111.616733635948,33.2195999971487), "POS14"),\</v>
+        <v>((-111.616733635948,33.3063435014256), "POS14"),\</v>
       </c>
     </row>
     <row r="21" spans="4:21" x14ac:dyDescent="0.25">
@@ -1004,22 +1041,22 @@
         <v>15</v>
       </c>
       <c r="Q21" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="R21" s="3">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="S21">
-        <f t="shared" si="0"/>
-        <v>-111.65131542396563</v>
+        <f t="shared" ref="S21" si="9">S$6+Q21*S$4+0.01</f>
+        <v>-111.61673363594844</v>
       </c>
       <c r="T21">
-        <f t="shared" si="1"/>
-        <v>33.219599997148705</v>
+        <f t="shared" ref="T21" si="10">T$6+R21*T$4+0.01</f>
+        <v>33.277428999999998</v>
       </c>
       <c r="U21" t="str">
-        <f t="shared" si="2"/>
-        <v>((-111.651315423966,33.2195999971487), "POS15"),\</v>
+        <f t="shared" ref="U21" si="11">_xlfn.CONCAT("((",S21,",",T21,"), ""POS",P21,"""),\")</f>
+        <v>((-111.616733635948,33.277429), "POS15"),\</v>
       </c>
     </row>
     <row r="22" spans="4:21" x14ac:dyDescent="0.25">
@@ -1027,22 +1064,22 @@
         <v>16</v>
       </c>
       <c r="Q22" s="3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="R22" s="3">
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="S22">
         <f t="shared" si="0"/>
-        <v>-111.68589721198281</v>
+        <v>-111.61673363594844</v>
       </c>
       <c r="T22">
         <f t="shared" si="1"/>
-        <v>33.219599997148705</v>
+        <v>33.248514498574352</v>
       </c>
       <c r="U22" t="str">
         <f t="shared" si="2"/>
-        <v>((-111.685897211983,33.2195999971487), "POS16"),\</v>
+        <v>((-111.616733635948,33.2485144985744), "POS16"),\</v>
       </c>
     </row>
     <row r="23" spans="4:21" x14ac:dyDescent="0.25">
@@ -1050,22 +1087,22 @@
         <v>17</v>
       </c>
       <c r="Q23" s="3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="R23" s="3">
-        <v>-6</v>
+        <v>-4</v>
       </c>
       <c r="S23">
         <f t="shared" si="0"/>
-        <v>-111.68589721198281</v>
+        <v>-111.61673363594844</v>
       </c>
       <c r="T23">
         <f t="shared" si="1"/>
-        <v>33.190685495723059</v>
+        <v>33.219599997148705</v>
       </c>
       <c r="U23" t="str">
         <f t="shared" si="2"/>
-        <v>((-111.685897211983,33.1906854957231), "POS17"),\</v>
+        <v>((-111.616733635948,33.2195999971487), "POS17"),\</v>
       </c>
     </row>
     <row r="24" spans="4:21" x14ac:dyDescent="0.25">
@@ -1073,25 +1110,511 @@
         <v>18</v>
       </c>
       <c r="Q24" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R24" s="3">
-        <v>-8</v>
+        <v>-4</v>
       </c>
       <c r="S24">
         <f t="shared" si="0"/>
-        <v>-111.68589721198281</v>
+        <v>-111.65131542396563</v>
       </c>
       <c r="T24">
         <f t="shared" si="1"/>
-        <v>33.161770994297413</v>
+        <v>33.219599997148705</v>
       </c>
       <c r="U24" t="str">
         <f t="shared" si="2"/>
-        <v>((-111.685897211983,33.1617709942974), "POS18"),\</v>
-      </c>
+        <v>((-111.651315423966,33.2195999971487), "POS18"),\</v>
+      </c>
+    </row>
+    <row r="25" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="P25" s="3">
+        <v>19</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>2</v>
+      </c>
+      <c r="R25" s="3">
+        <v>-4</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="0"/>
+        <v>-111.68589721198281</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="1"/>
+        <v>33.219599997148705</v>
+      </c>
+      <c r="U25" t="str">
+        <f t="shared" si="2"/>
+        <v>((-111.685897211983,33.2195999971487), "POS19"),\</v>
+      </c>
+    </row>
+    <row r="26" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="P26" s="3">
+        <v>20</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>2</v>
+      </c>
+      <c r="R26" s="3">
+        <v>-6</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="0"/>
+        <v>-111.68589721198281</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="1"/>
+        <v>33.190685495723059</v>
+      </c>
+      <c r="U26" t="str">
+        <f t="shared" si="2"/>
+        <v>((-111.685897211983,33.1906854957231), "POS20"),\</v>
+      </c>
+    </row>
+    <row r="27" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="P27" s="3">
+        <v>21</v>
+      </c>
+      <c r="Q27" s="3">
+        <v>2</v>
+      </c>
+      <c r="R27" s="3">
+        <v>-8</v>
+      </c>
+      <c r="S27">
+        <f t="shared" si="0"/>
+        <v>-111.68589721198281</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="1"/>
+        <v>33.161770994297413</v>
+      </c>
+      <c r="U27" t="str">
+        <f t="shared" si="2"/>
+        <v>((-111.685897211983,33.1617709942974), "POS21"),\</v>
+      </c>
+    </row>
+    <row r="31" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="S31" t="str">
+        <f>_xlfn.CONCAT(T6,",",S6)</f>
+        <v>33.267429,-111.730479</v>
+      </c>
+    </row>
+    <row r="32" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="S32" t="str">
+        <f t="shared" ref="S32:S52" si="12">_xlfn.CONCAT(T7,",",S7)</f>
+        <v>33.1617709942974,-111.824224364052</v>
+      </c>
+    </row>
+    <row r="33" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C33" s="7">
+        <v>4.291666666666667</v>
+      </c>
+      <c r="F33">
+        <v>33.2746</v>
+      </c>
+      <c r="G33">
+        <v>-111.8021</v>
+      </c>
+      <c r="H33" t="s">
+        <v>20</v>
+      </c>
+      <c r="S33" t="str">
+        <f t="shared" si="12"/>
+        <v>33.1906854957231,-111.824224364052</v>
+      </c>
+    </row>
+    <row r="34" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C34" s="7">
+        <v>4.333333333333333</v>
+      </c>
+      <c r="F34">
+        <v>33.251300000000001</v>
+      </c>
+      <c r="G34">
+        <v>-111.80459999999999</v>
+      </c>
+      <c r="H34" t="s">
+        <v>24</v>
+      </c>
+      <c r="S34" t="str">
+        <f t="shared" si="12"/>
+        <v>33.2195999971487,-111.824224364052</v>
+      </c>
+    </row>
+    <row r="35" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C35" s="7">
+        <v>25.041666666666668</v>
+      </c>
+      <c r="F35">
+        <v>33.335099999999997</v>
+      </c>
+      <c r="G35">
+        <v>-111.6497</v>
+      </c>
+      <c r="H35" t="s">
+        <v>25</v>
+      </c>
+      <c r="S35" t="str">
+        <f t="shared" si="12"/>
+        <v>33.2485144985744,-111.824224364052</v>
+      </c>
+    </row>
+    <row r="36" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C36" s="7">
+        <v>25.125</v>
+      </c>
+      <c r="F36">
+        <v>33.288400000000003</v>
+      </c>
+      <c r="G36">
+        <v>-111.6323</v>
+      </c>
+      <c r="H36" t="s">
+        <v>26</v>
+      </c>
+      <c r="S36" t="str">
+        <f t="shared" si="12"/>
+        <v>33.277429,-111.824224364052</v>
+      </c>
+    </row>
+    <row r="37" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C37" s="7">
+        <v>29.291666666666668</v>
+      </c>
+      <c r="F37">
+        <v>33.2926</v>
+      </c>
+      <c r="G37">
+        <v>-111.6193</v>
+      </c>
+      <c r="H37" t="s">
+        <v>27</v>
+      </c>
+      <c r="S37" t="str">
+        <f t="shared" si="12"/>
+        <v>33.3063435014256,-111.824224364052</v>
+      </c>
+    </row>
+    <row r="38" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C38" s="7">
+        <v>29.333333333333332</v>
+      </c>
+      <c r="F38">
+        <v>33.256700000000002</v>
+      </c>
+      <c r="G38">
+        <v>-111.5945</v>
+      </c>
+      <c r="H38" t="s">
+        <v>28</v>
+      </c>
+      <c r="S38" t="str">
+        <f t="shared" si="12"/>
+        <v>33.3352580028513,-111.824224364052</v>
+      </c>
+    </row>
+    <row r="39" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="S39" t="str">
+        <f t="shared" si="12"/>
+        <v>33.3352580028513,-111.789642576034</v>
+      </c>
+    </row>
+    <row r="40" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="S40" t="str">
+        <f t="shared" si="12"/>
+        <v>33.3352580028513,-111.755060788017</v>
+      </c>
+    </row>
+    <row r="41" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="S41" t="str">
+        <f t="shared" si="12"/>
+        <v>33.3352580028513,-111.720479</v>
+      </c>
+    </row>
+    <row r="42" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="S42" t="str">
+        <f t="shared" si="12"/>
+        <v>33.3352580028513,-111.685897211983</v>
+      </c>
+    </row>
+    <row r="43" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="S43" t="str">
+        <f t="shared" si="12"/>
+        <v>33.3352580028513,-111.651315423966</v>
+      </c>
+    </row>
+    <row r="44" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="S44" t="str">
+        <f t="shared" si="12"/>
+        <v>33.3352580028513,-111.616733635948</v>
+      </c>
+    </row>
+    <row r="45" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="S45" t="str">
+        <f t="shared" si="12"/>
+        <v>33.3063435014256,-111.616733635948</v>
+      </c>
+    </row>
+    <row r="46" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="S46" t="str">
+        <f t="shared" si="12"/>
+        <v>33.277429,-111.616733635948</v>
+      </c>
+    </row>
+    <row r="47" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C47" s="7"/>
+      <c r="D47" t="s">
+        <v>29</v>
+      </c>
+      <c r="E47" t="s">
+        <v>21</v>
+      </c>
+      <c r="F47">
+        <v>33.331400000000002</v>
+      </c>
+      <c r="G47" t="s">
+        <v>22</v>
+      </c>
+      <c r="H47">
+        <v>-111.7671</v>
+      </c>
+      <c r="J47" t="s">
+        <v>23</v>
+      </c>
+      <c r="K47" t="str">
+        <f>_xlfn.CONCAT(F47:H47)</f>
+        <v>33.3314,-111.7671</v>
+      </c>
+      <c r="S47" t="str">
+        <f t="shared" si="12"/>
+        <v>33.2485144985744,-111.616733635948</v>
+      </c>
+    </row>
+    <row r="48" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C48" s="7"/>
+      <c r="D48" t="s">
+        <v>29</v>
+      </c>
+      <c r="E48" t="s">
+        <v>21</v>
+      </c>
+      <c r="F48">
+        <v>33.319299999999998</v>
+      </c>
+      <c r="G48" t="s">
+        <v>22</v>
+      </c>
+      <c r="H48">
+        <v>-111.7709</v>
+      </c>
+      <c r="J48" t="s">
+        <v>23</v>
+      </c>
+      <c r="K48" t="str">
+        <f t="shared" ref="K48:K54" si="13">_xlfn.CONCAT(F48:H48)</f>
+        <v>33.3193,-111.7709</v>
+      </c>
+      <c r="S48" t="str">
+        <f t="shared" si="12"/>
+        <v>33.2195999971487,-111.616733635948</v>
+      </c>
+    </row>
+    <row r="49" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C49" s="7"/>
+      <c r="D49" t="s">
+        <v>30</v>
+      </c>
+      <c r="E49" t="s">
+        <v>21</v>
+      </c>
+      <c r="F49">
+        <v>33.2821</v>
+      </c>
+      <c r="G49" t="s">
+        <v>22</v>
+      </c>
+      <c r="H49">
+        <v>-111.79130000000001</v>
+      </c>
+      <c r="J49" t="s">
+        <v>23</v>
+      </c>
+      <c r="K49" t="str">
+        <f t="shared" si="13"/>
+        <v>33.2821,-111.7913</v>
+      </c>
+      <c r="S49" t="str">
+        <f t="shared" si="12"/>
+        <v>33.2195999971487,-111.651315423966</v>
+      </c>
+    </row>
+    <row r="50" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C50" s="7"/>
+      <c r="D50" t="s">
+        <v>30</v>
+      </c>
+      <c r="E50" t="s">
+        <v>21</v>
+      </c>
+      <c r="F50">
+        <v>33.279400000000003</v>
+      </c>
+      <c r="G50" t="s">
+        <v>22</v>
+      </c>
+      <c r="H50">
+        <v>-111.795</v>
+      </c>
+      <c r="J50" t="s">
+        <v>23</v>
+      </c>
+      <c r="K50" t="str">
+        <f t="shared" si="13"/>
+        <v>33.2794,-111.795</v>
+      </c>
+      <c r="S50" t="str">
+        <f t="shared" si="12"/>
+        <v>33.2195999971487,-111.685897211983</v>
+      </c>
+    </row>
+    <row r="51" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C51" s="7"/>
+      <c r="D51" t="s">
+        <v>31</v>
+      </c>
+      <c r="E51" t="s">
+        <v>21</v>
+      </c>
+      <c r="F51">
+        <v>33.281199999999998</v>
+      </c>
+      <c r="G51" t="s">
+        <v>22</v>
+      </c>
+      <c r="H51">
+        <v>-111.623</v>
+      </c>
+      <c r="J51" t="s">
+        <v>23</v>
+      </c>
+      <c r="K51" t="str">
+        <f t="shared" si="13"/>
+        <v>33.2812,-111.623</v>
+      </c>
+      <c r="S51" t="str">
+        <f t="shared" si="12"/>
+        <v>33.1906854957231,-111.685897211983</v>
+      </c>
+    </row>
+    <row r="52" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C52" s="7"/>
+      <c r="D52" t="s">
+        <v>31</v>
+      </c>
+      <c r="E52" t="s">
+        <v>21</v>
+      </c>
+      <c r="F52">
+        <v>33.319299999999998</v>
+      </c>
+      <c r="G52" t="s">
+        <v>22</v>
+      </c>
+      <c r="H52">
+        <v>-111.6677</v>
+      </c>
+      <c r="J52" t="s">
+        <v>23</v>
+      </c>
+      <c r="K52" t="str">
+        <f t="shared" si="13"/>
+        <v>33.3193,-111.6677</v>
+      </c>
+      <c r="S52" t="str">
+        <f t="shared" si="12"/>
+        <v>33.1617709942974,-111.685897211983</v>
+      </c>
+    </row>
+    <row r="53" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C53" s="7"/>
+      <c r="D53" t="s">
+        <v>20</v>
+      </c>
+      <c r="E53" t="s">
+        <v>21</v>
+      </c>
+      <c r="F53">
+        <v>33.277999999999999</v>
+      </c>
+      <c r="G53" t="s">
+        <v>22</v>
+      </c>
+      <c r="H53">
+        <v>-111.79559999999999</v>
+      </c>
+      <c r="J53" t="s">
+        <v>23</v>
+      </c>
+      <c r="K53" t="str">
+        <f t="shared" si="13"/>
+        <v>33.278,-111.7956</v>
+      </c>
+      <c r="S53" t="str">
+        <f>_xlfn.CONCAT(F33,",",G33)</f>
+        <v>33.2746,-111.8021</v>
+      </c>
+    </row>
+    <row r="54" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C54" s="7"/>
+      <c r="D54" t="s">
+        <v>20</v>
+      </c>
+      <c r="E54" t="s">
+        <v>21</v>
+      </c>
+      <c r="F54">
+        <v>33.273800000000001</v>
+      </c>
+      <c r="G54" t="s">
+        <v>22</v>
+      </c>
+      <c r="H54">
+        <v>-111.8018</v>
+      </c>
+      <c r="J54" t="s">
+        <v>23</v>
+      </c>
+      <c r="K54" t="str">
+        <f t="shared" si="13"/>
+        <v>33.2738,-111.8018</v>
+      </c>
+    </row>
+    <row r="55" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C55" s="7"/>
+    </row>
+    <row r="56" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C56" s="7"/>
+    </row>
+    <row r="57" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C57" s="7"/>
+    </row>
+    <row r="58" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C58" s="7"/>
+    </row>
+    <row r="59" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C59" s="7"/>
+    </row>
+    <row r="60" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C60" s="7"/>
     </row>
   </sheetData>
+  <sortState ref="D47:F58">
+    <sortCondition ref="D47"/>
+  </sortState>
   <mergeCells count="2">
     <mergeCell ref="Q5:R5"/>
     <mergeCell ref="S5:T5"/>

</xml_diff>